<commit_message>
update avancement listing page
</commit_message>
<xml_diff>
--- a/Livrables/listing_page.xlsx
+++ b/Livrables/listing_page.xlsx
@@ -308,13 +308,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,7 +604,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,16 +640,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -660,13 +660,13 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="16" t="s">
+      <c r="E3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H3" s="2"/>
@@ -680,13 +680,13 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="16" t="s">
+      <c r="E4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -705,10 +705,10 @@
       <c r="E5" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -724,13 +724,13 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="16" t="s">
+      <c r="E6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -738,16 +738,16 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -758,13 +758,13 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="16" t="s">
+      <c r="E8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -780,13 +780,13 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="16" t="s">
+      <c r="E9" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -802,13 +802,13 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="16" t="s">
+      <c r="E10" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -827,10 +827,10 @@
       <c r="E11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="16" t="s">
+      <c r="F11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -846,13 +846,13 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="16" t="s">
+      <c r="E12" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -868,13 +868,13 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="16" t="s">
+      <c r="E13" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -890,13 +890,13 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="16" t="s">
+      <c r="E14" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H14" s="6" t="s">
@@ -904,16 +904,16 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -924,13 +924,13 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="16" t="s">
+      <c r="E16" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -949,10 +949,10 @@
       <c r="E17" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="16" t="s">
+      <c r="F17" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -971,10 +971,10 @@
       <c r="E18" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="16" t="s">
+      <c r="F18" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -993,10 +993,10 @@
       <c r="E19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" s="16" t="s">
+      <c r="F19" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -1015,10 +1015,10 @@
       <c r="E20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="16" t="s">
+      <c r="F20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -1037,10 +1037,10 @@
       <c r="E21" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="16" t="s">
+      <c r="F21" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -1056,9 +1056,9 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16" t="s">
+      <c r="E22" s="12"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H22" s="2" t="s">

</xml_diff>

<commit_message>
create States + update listing
</commit_message>
<xml_diff>
--- a/Livrables/listing_page.xlsx
+++ b/Livrables/listing_page.xlsx
@@ -604,7 +604,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +683,7 @@
       <c r="E4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="15" t="s">
@@ -705,7 +705,7 @@
       <c r="E5" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G5" s="15" t="s">
@@ -849,7 +849,7 @@
       <c r="E12" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="15" t="s">
@@ -949,7 +949,7 @@
       <c r="E17" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G17" s="15" t="s">
@@ -971,7 +971,7 @@
       <c r="E18" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G18" s="15" t="s">
@@ -993,7 +993,7 @@
       <c r="E19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G19" s="15" t="s">
@@ -1015,7 +1015,7 @@
       <c r="E20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G20" s="15" t="s">
@@ -1037,7 +1037,7 @@
       <c r="E21" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G21" s="15" t="s">
@@ -1057,7 +1057,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="15"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="15" t="s">
         <v>45</v>
       </c>

</xml_diff>